<commit_message>
updated data sources list hopefully
</commit_message>
<xml_diff>
--- a/data/data-sources.xlsx
+++ b/data/data-sources.xlsx
@@ -16,7 +16,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>Useful</t>
+  </si>
   <si>
     <t>Names</t>
   </si>
@@ -28,18 +31,107 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Victorian Road Crash Data</t>
+  </si>
+  <si>
+    <t>DOT/DTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allll the crashes in different data sets... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">arcGIS visualisation tool: https://vicroadsopendata-vicroadsmaps.opendata.arcgis.com/datasets/25e6727f89f2472aa7b044a3ae730b9a_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic Count Location</t>
+  </si>
+  <si>
+    <t>VicRoads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This dataset contains the location, GPS coordinates and textural description, of all traffic counts conducted by VicRoads over the past 20+ years</t>
+  </si>
+  <si>
+    <t>https://discover.data.vic.gov.au/dataset/traffic-count-locations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic Signals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location of all traffic 'signals' nb includes pedestrian crossings with lights</t>
+  </si>
+  <si>
+    <t>https://discover.data.vic.gov.au/dataset/traffic-lights1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed Signs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A spatial dataset (point) showing the location of every speed sign across Victoria including attributes such as Road Name, Sign Size, Type, Speed Value, Bearing and Direction. Some speed signs have varying values depending on the time of the day which is also incorporated into this dataset.</t>
+  </si>
+  <si>
+    <t>https://discover.data.vic.gov.au/dataset/speed-signs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic Signal Volume Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each file contains all of the 15 minute traffic volumes for traffic signals by detector for years from 2014. A detector is a loop of wire installed into the road surface and is activated when a vehicle passes over it and sends a pulse to the traffic signal.</t>
+  </si>
+  <si>
+    <t>https://discover.data.vic.gov.au/dataset/traffic-signal-volume-data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic Signal Configuration Data Sheets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic Signal Configuration Data Sheets, also known as Op Sheets, are the operational design criteria for the traffic signals across Victoria. Each traffic signal requires this information for signal phasing. </t>
+  </si>
+  <si>
+    <t>https://discover.data.vic.gov.au/dataset/traffic-signal-configuration-data-sheets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VicRoads Turning Movement Volume Surveys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed Zones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane Use Management Signals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* API. data set is too large to download and make available ... </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple Variable Electronic Speed Signs Live</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.000000"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10.500000"/>
+      <color indexed="64"/>
+      <name val="Open Sans"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,8 +154,29 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,31 +687,174 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.421875"/>
-    <col customWidth="1" min="3" max="3" width="13.140625"/>
+    <col min="1" max="1" style="1" width="9.140625"/>
+    <col customWidth="1" min="2" max="2" style="1" width="23.421875"/>
+    <col customWidth="1" min="3" max="3" style="1" width="22.57421875"/>
+    <col customWidth="1" min="4" max="4" style="2" width="71.421875"/>
+    <col min="5" max="5" style="1" width="9.140625"/>
+    <col min="6" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" ht="28.5">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" ht="57">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" ht="42.75">
+      <c r="A7" s="1"/>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" ht="42.75">
+      <c r="A8" s="1"/>
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75">
+      <c r="A10" s="1"/>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75">
+      <c r="A11" s="1"/>
+      <c r="B11" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75">
+      <c r="A13" s="1"/>
+      <c r="B13" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E4"/>
+    <hyperlink r:id="rId2" ref="E5"/>
+    <hyperlink r:id="rId3" ref="E6"/>
+    <hyperlink r:id="rId4" ref="E7"/>
+    <hyperlink r:id="rId5" ref="E8"/>
+  </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>